<commit_message>
Update notes columns specifications, add notes column to component table
</commit_message>
<xml_diff>
--- a/BCB420-2019-System-XXXXX-0.0.xlsx
+++ b/BCB420-2019-System-XXXXX-0.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24709"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="-23780" windowWidth="31420" windowHeight="23380"/>
+    <workbookView xWindow="3220" yWindow="-23960" windowWidth="31420" windowHeight="23380" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="system" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>name</t>
   </si>
@@ -83,9 +83,6 @@
     <t>uniprot</t>
   </si>
   <si>
-    <t>Brief description of function</t>
-  </si>
-  <si>
     <t>Short (5-letter code) or gene symbol</t>
   </si>
   <si>
@@ -108,6 +105,12 @@
   </si>
   <si>
     <t>(protein | RNA | lipid | metabolite)</t>
+  </si>
+  <si>
+    <t>Brief description of the functionality that the component contributes to the system</t>
+  </si>
+  <si>
+    <t>Brief description of  properties that are  important to the component regardless of its role in the system</t>
   </si>
 </sst>
 </file>
@@ -180,8 +183,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -218,7 +223,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -230,6 +235,7 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -241,6 +247,7 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -535,7 +542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -549,7 +556,7 @@
   <sheetData>
     <row r="1" spans="1:17" s="4" customFormat="1" ht="24">
       <c r="A1" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>6</v>
@@ -604,7 +611,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F62"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -613,29 +620,29 @@
     <col min="2" max="2" width="20.83203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="9.1640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="15" style="3" customWidth="1"/>
-    <col min="5" max="5" width="22.1640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="31" style="3" customWidth="1"/>
     <col min="7" max="16" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="4" customFormat="1" ht="36">
       <c r="A1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1">
@@ -655,7 +662,7 @@
         <v>4</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -683,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -693,12 +700,14 @@
     <col min="2" max="2" width="17.83203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="22.1640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" style="3" customWidth="1"/>
-    <col min="5" max="16" width="8.83203125" style="3"/>
+    <col min="5" max="6" width="8.83203125" style="3"/>
+    <col min="7" max="7" width="26.5" style="3" customWidth="1"/>
+    <col min="8" max="16" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="24">
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="36">
       <c r="A1" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>6</v>
@@ -707,13 +716,16 @@
         <v>18</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>16</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1">
@@ -730,12 +742,14 @@
         <v>17</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>

</xml_diff>